<commit_message>
implement phân công giảng dạy
</commit_message>
<xml_diff>
--- a/mockupData_python/student_info_with_mockup.xlsx
+++ b/mockupData_python/student_info_with_mockup.xlsx
@@ -584,108 +584,92 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Uông Đình</t>
+          <t>Đào Đức</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dương</t>
+          <t>Nguyễn</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>03/16/1999</t>
+          <t>08/08/2005</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Pà Thẻn</t>
+          <t>HMông</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>09/01/2024</t>
+          <t>09/17/2024</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0850884960</t>
+          <t>0935853935</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Hồ Chí Minh</t>
+          <t>Hà Nam</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Bùi Chu Hữu</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>08/13/1959</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>0718452336</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Sales Representative</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Vũ Chu Hữu</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>03/02/1994</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>0940162254</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>Thợ xây</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
+          <t>Ông bà</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Vũ Trần Quốc</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>12/26/1955</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>0783959296</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Nông dân</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -701,22 +685,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Đinh Đức</t>
+          <t>Thạch Đình</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Vũ</t>
+          <t>Dương</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>01/09/2005</t>
+          <t>05/03/2004</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -726,67 +710,83 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Brau</t>
+          <t>Chứt</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>09/04/2024</t>
+          <t>09/21/2024</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0740497042</t>
+          <t>0905412458</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Bến Tre</t>
+          <t>Đồng Nai</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Họ hàng</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>Hoàng Ngô Đình</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>07/13/1956</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>0838043827</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>Chuyên viên tư vấn tuyển sinh</t>
-        </is>
-      </c>
+          <t>Không</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Phạm Trịnh Đình</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>02/10/1967</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>0853592077</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Giám đốc kinh doanh</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Dương Đoàn Hồng</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>08/18/1967</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>0851547006</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Luật sư</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -802,22 +802,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Phùng Đức</t>
+          <t>Tôn Hồng</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Đặng</t>
+          <t>Dương</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>04/29/2001</t>
+          <t>07/16/2006</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -827,22 +827,22 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Ơ Đu</t>
+          <t>La Chi</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>08/31/2024</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0935849788</t>
+          <t>0362206472</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Tuyên Quang</t>
+          <t>Sóc Trăng</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -870,22 +870,22 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr">
         <is>
-          <t>Đặng Tôn Văn</t>
+          <t>Dương Đinh Đức</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>02/19/1968</t>
+          <t>02/20/1961</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>0892304084</t>
+          <t>0870383060</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>Biên dịch viên</t>
+          <t>Điều Dưỡng</t>
         </is>
       </c>
     </row>
@@ -903,12 +903,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Phùng Đình</t>
+          <t>Trịnh Thành</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -918,7 +918,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>07/06/2002</t>
+          <t>09/19/2006</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -928,27 +928,27 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Thổ</t>
+          <t>La Ha</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>09/27/2024</t>
+          <t>09/20/2024</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0837625315</t>
+          <t>0883987305</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Vĩnh Long</t>
+          <t>Long An</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -961,28 +961,44 @@
           <t>Không</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Bùi Thi Văn</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>06/25/1965</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>0387472078</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Trưởng phòng kinh doanh</t>
+        </is>
+      </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Bùi Lưu Thành</t>
+          <t>Trần Lý Hữu</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>12/27/1963</t>
+          <t>04/08/1957</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>0847051460</t>
+          <t>0343306901</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>Kỹ sư giám sát</t>
+          <t>Thực Tập</t>
         </is>
       </c>
       <c r="X5" t="inlineStr"/>
@@ -1004,47 +1020,47 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Vũ Văn</t>
+          <t>Thi Thành</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Lê</t>
+          <t>Hoàng</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>03/04/2001</t>
+          <t>03/21/2001</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Pà Thẻn</t>
+          <t>Tày</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>08/31/2024</t>
+          <t>10/02/2024</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0846296996</t>
+          <t>0813046262</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Thừa Thiên Huế</t>
+          <t>Bạc Liêu</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -1064,22 +1080,22 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Phạm Quách Thành</t>
+          <t>Bùi Thạch Đình</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>04/15/1972</t>
+          <t>07/26/1970</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>0867511888</t>
+          <t>0953588463</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>Kỹ sư nông nghiệp</t>
+          <t>DevOps Engineer</t>
         </is>
       </c>
       <c r="T6" t="inlineStr"/>
@@ -1105,22 +1121,22 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Thạch Thị</t>
+          <t>Tôn Hữu</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dương</t>
+          <t>Nguyễn</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>08/16/2005</t>
+          <t>09/22/2000</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1130,22 +1146,22 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Pà Thẻn</t>
+          <t>La Chi</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>09/20/2024</t>
+          <t>10/02/2024</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0320767897</t>
+          <t>0940828625</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Lạng Sơn</t>
+          <t>Hà Giang</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1160,7 +1176,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Họ hàng</t>
+          <t>Ông bà</t>
         </is>
       </c>
       <c r="P7" t="inlineStr"/>
@@ -1173,22 +1189,22 @@
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr">
         <is>
-          <t>Mai Trịnh Minh</t>
+          <t>Vũ Hoàng Thành</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>01/12/1993</t>
+          <t>04/25/1968</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>0825487073</t>
+          <t>0902633593</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>Nhân viên hành chính</t>
+          <t>Trưởng phòng kinh doanh</t>
         </is>
       </c>
     </row>
@@ -1206,22 +1222,22 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Tiêu Thị</t>
+          <t>Hứa Thành</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Lê</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>06/15/2002</t>
+          <t>12/14/1998</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1231,22 +1247,22 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Brau</t>
+          <t>Gia Rai</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>09/06/2024</t>
+          <t>10/06/2024</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0787396747</t>
+          <t>0842594298</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Quảng Ngãi</t>
+          <t>Đồng Tháp</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1256,42 +1272,42 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Anh chị</t>
         </is>
       </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>Phạm Vương Đức</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>11/28/1989</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>0311043011</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>Sales Representative</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>Hoàng Trịnh Thị</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>09/26/1980</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>0914224251</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>Dược sĩ</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -1307,22 +1323,22 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Hứa Đình</t>
+          <t>Sơn Hữu</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Hoàng</t>
+          <t>Vũ</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>05/08/2005</t>
+          <t>04/30/2004</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1332,77 +1348,61 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Mảng</t>
+          <t>HMông</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>09/14/2024</t>
+          <t>09/26/2024</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0906953239</t>
+          <t>0857313705</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Hà Giang</t>
+          <t>Sơn La</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
+          <t>Không</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
           <t>Có</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>Có</t>
-        </is>
-      </c>
       <c r="O9" t="inlineStr">
         <is>
           <t>Không</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>Bùi Đinh Văn</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>05/11/1989</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>0717414275</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>Kỹ sư phần mềm</t>
-        </is>
-      </c>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Nguyễn Đoàn Hồng</t>
+          <t>Trần Phí Văn</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>12/02/1970</t>
+          <t>08/15/1978</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>0947085171</t>
+          <t>0321545698</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>Kiến trúc sư</t>
+          <t>Project Manager</t>
         </is>
       </c>
       <c r="X9" t="inlineStr"/>
@@ -1424,22 +1424,22 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Vũ Đình</t>
+          <t>Sơn Quốc</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Mai</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>01/04/2006</t>
+          <t>12/03/1999</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1449,22 +1449,22 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Khơ Mú</t>
+          <t>Chu Ru</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>09/22/2024</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0969669052</t>
+          <t>0764005568</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Phú Yên</t>
+          <t>Đồng Tháp</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1474,42 +1474,42 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Anh chị</t>
         </is>
       </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>Mai Đinh Thành</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>01/28/1975</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>0905346741</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>Chuyên viên bảo mật</t>
-        </is>
-      </c>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>Bùi Đào Quốc</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>03/17/1970</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>0819802122</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>Công nhân sản xuất</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -1525,47 +1525,47 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Hứa Hữu</t>
+          <t>Mai Thị</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Bùi</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>08/19/2000</t>
+          <t>11/28/2001</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Xtiêng</t>
+          <t>Rơ Măm</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>09/16/2024</t>
+          <t>10/01/2024</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0722582860</t>
+          <t>0372180819</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Bến Tre</t>
+          <t>Đà Nẵng</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1589,22 +1589,22 @@
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr">
         <is>
-          <t>Dương Vương Thị</t>
+          <t>Mai Quách Đình</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>09/26/1959</t>
+          <t>09/06/1957</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>0310191746</t>
+          <t>0338749977</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>Thực tập sinh giáo dục</t>
+          <t>Nông dân</t>
         </is>
       </c>
       <c r="X11" t="inlineStr"/>
@@ -1626,47 +1626,47 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Lý Đình</t>
+          <t>Trương Thành</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Bùi</t>
+          <t>Phạm</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>03/15/2002</t>
+          <t>06/11/2001</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Mảng</t>
+          <t>Ê Đê</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>09/26/2024</t>
+          <t>09/12/2024</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>0311195657</t>
+          <t>0739457416</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Nam Định</t>
+          <t>Tuyên Quang</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1686,22 +1686,22 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Vũ Lý Quốc</t>
+          <t>Phạm Đào Minh</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>12/03/1965</t>
+          <t>05/16/1991</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>0912853776</t>
+          <t>0899926677</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>Luật sư</t>
+          <t>Thực Tập</t>
         </is>
       </c>
       <c r="T12" t="inlineStr"/>
@@ -1727,12 +1727,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Trịnh Thành</t>
+          <t>Sơn Minh</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>03/21/2005</t>
+          <t>06/11/2000</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1752,77 +1752,61 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Ơ Đu</t>
+          <t>Ê Đê</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>09/25/2024</t>
+          <t>09/28/2024</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>0738880098</t>
+          <t>0813638623</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Tây Ninh</t>
+          <t>Hòa Bình</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
+          <t>Không</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
           <t>Có</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>Có</t>
-        </is>
-      </c>
       <c r="O13" t="inlineStr">
         <is>
           <t>Không</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>Dương Huỳnh Văn</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>11/09/1975</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>0765791557</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>Nhân viên kinh doanh</t>
-        </is>
-      </c>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr">
         <is>
-          <t>Trần Hà Hữu</t>
+          <t>Mai Từ Văn</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>03/04/1991</t>
+          <t>01/24/1991</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>0383330320</t>
+          <t>0779498988</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>Điều Dưỡng</t>
+          <t>Nhà tư vấn tài chính</t>
         </is>
       </c>
       <c r="X13" t="inlineStr"/>
@@ -1844,47 +1828,47 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Vũ Văn</t>
+          <t>Hoàng Hồng</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Mai</t>
+          <t>Trần</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>06/23/2006</t>
+          <t>10/20/1999</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Hoa</t>
+          <t>La Hu</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>09/06/2024</t>
+          <t>09/29/2024</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>0359759296</t>
+          <t>0726796542</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Sơn La</t>
+          <t>Trà Vinh</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1894,42 +1878,42 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Anh chị</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr">
-        <is>
-          <t>Trần Uông Thị</t>
-        </is>
-      </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>03/06/1976</t>
-        </is>
-      </c>
-      <c r="Z14" t="inlineStr">
-        <is>
-          <t>0371629853</t>
-        </is>
-      </c>
-      <c r="AA14" t="inlineStr">
-        <is>
-          <t>Tư vấn khách hàng</t>
-        </is>
-      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Trần Nguyễn Thị</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>10/30/1977</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>0352859536</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>Nhân viên hành chính</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -1945,22 +1929,22 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Thạch Đức</t>
+          <t>Lương Thị</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Bùi</t>
+          <t>Lê</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>04/28/2003</t>
+          <t>12/20/1999</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1970,7 +1954,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Chu Ru</t>
+          <t>Ngái</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1980,17 +1964,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>0811906937</t>
+          <t>0750274591</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Điện Biên</t>
+          <t>Vĩnh Long</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -2003,28 +1987,44 @@
           <t>Không</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Hoàng Hứa Đức</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>08/04/1985</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>0951624806</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Nhân viên nhà hàng</t>
+        </is>
+      </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>Phạm Hà Văn</t>
+          <t>Vũ Đinh Quốc</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>02/14/1976</t>
+          <t>05/07/1972</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>0900469863</t>
+          <t>0390886271</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>Giám đốc kinh doanh</t>
+          <t>Nhân viên khách sạn</t>
         </is>
       </c>
       <c r="X15" t="inlineStr"/>
@@ -2046,22 +2046,22 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Đặng Hồng</t>
+          <t>Trần Quốc</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Dương</t>
+          <t>Bùi</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>03/20/1999</t>
+          <t>09/29/2001</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -2071,22 +2071,22 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Pu Ko</t>
+          <t>Ngái</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>09/16/2024</t>
+          <t>09/12/2024</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>0732125029</t>
+          <t>0983934332</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Sơn La</t>
+          <t>Lào Cai</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -2096,42 +2096,42 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Ông bà</t>
         </is>
       </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>Phạm Phan Quốc</t>
-        </is>
-      </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>05/04/1985</t>
-        </is>
-      </c>
-      <c r="V16" t="inlineStr">
-        <is>
-          <t>0800023956</t>
-        </is>
-      </c>
-      <c r="W16" t="inlineStr">
-        <is>
-          <t>Digital Marketer</t>
-        </is>
-      </c>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>Phạm Sơn Đức</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>04/06/1958</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>0847369063</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>Sales Representative</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -2147,22 +2147,22 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Đinh Quốc</t>
+          <t>Hà Thị</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Đặng</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>09/06/2002</t>
+          <t>04/25/2006</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -2172,32 +2172,32 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Hoa</t>
+          <t>Brau</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>09/18/2024</t>
+          <t>09/16/2024</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>0806416690</t>
+          <t>0866056539</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Quảng Ngãi</t>
+          <t>Gia Lai</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -2205,30 +2205,30 @@
           <t>Không</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>Phạm Từ Đức</t>
-        </is>
-      </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>09/22/1981</t>
-        </is>
-      </c>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t>0879880570</t>
-        </is>
-      </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>Chuyên viên nhân sự</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Lê Nguyễn Quốc</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>10/07/1956</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>0324321748</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr"/>
@@ -2248,22 +2248,22 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Phí Đình</t>
+          <t>Uông Văn</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Vũ</t>
+          <t>Mai</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>09/23/2001</t>
+          <t>03/01/2004</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -2273,27 +2273,27 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>La Chí</t>
+          <t>Lô Lô</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>09/07/2024</t>
+          <t>10/09/2024</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>0727032680</t>
+          <t>0728728202</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Bình Phước</t>
+          <t>Hải Dương</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -2303,37 +2303,37 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>Bùi Trịnh Minh</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>10/07/1988</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>0752871644</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>Chuyên viên phân tích thị trường</t>
-        </is>
-      </c>
+          <t>Ông bà</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
-      <c r="Z18" t="inlineStr"/>
-      <c r="AA18" t="inlineStr"/>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>Lê Khương Thị</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>07/07/1988</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>0813791862</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>Chuyên viên nhân sự</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -2349,22 +2349,22 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Nguyễn Đình</t>
+          <t>Hứa Đức</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Hoàng</t>
+          <t>Phạm</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>02/03/2005</t>
+          <t>06/01/2005</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -2374,22 +2374,22 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Rơ Măm</t>
+          <t>Ê Đê</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>09/27/2024</t>
+          <t>09/12/2024</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>0722170680</t>
+          <t>0720408602</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Thái Nguyên</t>
+          <t>Khánh Hòa</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -2409,42 +2409,42 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Phạm Thái Minh</t>
+          <t>Đặng Tôn Hữu</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>04/19/1972</t>
+          <t>05/12/1974</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>0796058662</t>
+          <t>0379728629</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>Sales Representative</t>
+          <t>Quản lý sản xuất</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>Lê Vương Đức</t>
+          <t>Mai Phí Hữu</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>03/03/1990</t>
+          <t>05/09/1990</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>0367235852</t>
+          <t>0795949384</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>Quản lý sản xuất</t>
+          <t>Chuyên viên bán hàng trực tuyến</t>
         </is>
       </c>
       <c r="X19" t="inlineStr"/>
@@ -2466,47 +2466,47 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Vũ Quốc</t>
+          <t>Nghiêm Hồng</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Dương</t>
+          <t>Trần</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>07/23/2000</t>
+          <t>12/01/1999</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Cống</t>
+          <t>La Hu</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>09/22/2024</t>
+          <t>10/03/2024</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>0916715361</t>
+          <t>0359534483</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Đà Nẵng</t>
+          <t>Hồ Chí Minh</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Anh chị</t>
+          <t>Ông bà</t>
         </is>
       </c>
       <c r="P20" t="inlineStr"/>
@@ -2534,22 +2534,22 @@
       <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr">
         <is>
-          <t>Đặng Sơn Thành</t>
+          <t>Mai Khương Đình</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>10/16/1972</t>
+          <t>02/18/1972</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>0995933708</t>
+          <t>0329164887</t>
         </is>
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>Nông dân</t>
+          <t>Kỹ sư nông nghiệp</t>
         </is>
       </c>
     </row>
@@ -2567,22 +2567,22 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Trương Văn</t>
+          <t>Đào Hồng</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Lê</t>
+          <t>Dương</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>10/09/2005</t>
+          <t>02/01/2000</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -2592,27 +2592,27 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>HMông</t>
+          <t>La Hu</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>09/15/2024</t>
+          <t>09/21/2024</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>0389667311</t>
+          <t>0701897310</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Bến Tre</t>
+          <t>Bắc Ninh</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2625,28 +2625,44 @@
           <t>Không</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Nguyễn Lương Hữu</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>07/03/1977</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>0804202278</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Marketing Manager</t>
+        </is>
+      </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>Phạm Thái Hữu</t>
+          <t>Phạm Tạ Văn</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>10/13/1969</t>
+          <t>11/13/1967</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>0805050973</t>
+          <t>0382547327</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>Kỹ sư xây dựng</t>
+          <t>Trưởng phòng kinh doanh</t>
         </is>
       </c>
       <c r="X21" t="inlineStr"/>
@@ -2668,47 +2684,47 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Tôn Minh</t>
+          <t>Vương Hữu</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Mai</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>03/01/2004</t>
+          <t>01/26/2001</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Pu Péo</t>
+          <t>La Ha</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>09/12/2024</t>
+          <t>09/27/2024</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>0945554947</t>
+          <t>0733201931</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Bạc Liêu</t>
+          <t>Hải Dương</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -2728,22 +2744,22 @@
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Hoàng Trịnh Văn</t>
+          <t>Lê Hoàng Quốc</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>12/31/1991</t>
+          <t>10/21/1966</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>0834616277</t>
+          <t>0963947872</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Dược sĩ</t>
+          <t>Nhà tư vấn tài chính</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
@@ -2769,22 +2785,22 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Tô Thành</t>
+          <t>Phan Văn</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Phạm</t>
+          <t>Đặng</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>10/21/1999</t>
+          <t>08/10/1999</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2794,22 +2810,22 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Bố Y</t>
+          <t>Thổ</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>09/27/2024</t>
+          <t>09/17/2024</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>0350847512</t>
+          <t>0758956176</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Cà Mau</t>
+          <t>Hải Phòng</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2819,7 +2835,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
@@ -2829,28 +2845,44 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Vũ Uông Văn</t>
+          <t>Phạm Chu Thị</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>12/17/1954</t>
+          <t>03/30/1978</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>0711763937</t>
+          <t>0798167060</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
         <is>
+          <t>Kiến trúc sư phần mềm</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Vũ Võ Văn</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>10/08/1987</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>0881349036</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
           <t>Giám đốc kinh doanh</t>
         </is>
       </c>
-      <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr"/>
-      <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr"/>
@@ -2870,22 +2902,22 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Đinh Minh</t>
+          <t>Trịnh Minh</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Đặng</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>04/17/2000</t>
+          <t>11/22/1998</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2895,77 +2927,61 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Xtiêng</t>
+          <t>Khơ Mú</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>09/05/2024</t>
+          <t>09/13/2024</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>0366102702</t>
+          <t>0900191883</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Bến Tre</t>
+          <t>Bạc Liêu</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
+          <t>Không</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
           <t>Có</t>
         </is>
       </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>Có</t>
-        </is>
-      </c>
       <c r="O24" t="inlineStr">
         <is>
           <t>Không</t>
         </is>
       </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>Đặng Khương Đức</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>07/27/1969</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>0889711614</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>Quản lý sản xuất</t>
-        </is>
-      </c>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr">
         <is>
-          <t>Trần Phí Minh</t>
+          <t>Đặng Tiêu Quốc</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>05/04/1977</t>
+          <t>04/03/1964</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>0763446114</t>
+          <t>0388757608</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>Thợ xây</t>
+          <t>Công nhân sản xuất</t>
         </is>
       </c>
       <c r="X24" t="inlineStr"/>
@@ -2987,47 +3003,47 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Đinh Đình</t>
+          <t>Phạm Hồng</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Bùi</t>
+          <t>Phạm</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>04/15/2006</t>
+          <t>02/02/2003</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Cơ Ho</t>
+          <t>La Hủ</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>09/02/2024</t>
+          <t>10/09/2024</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>0864930083</t>
+          <t>0345912258</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Bạc Liêu</t>
+          <t>Hòa Bình</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -3037,42 +3053,42 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Họ hàng</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
-      <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
-      <c r="W25" t="inlineStr"/>
-      <c r="X25" t="inlineStr">
-        <is>
-          <t>Mai Hoàng Đình</t>
-        </is>
-      </c>
-      <c r="Y25" t="inlineStr">
-        <is>
-          <t>10/13/1965</t>
-        </is>
-      </c>
-      <c r="Z25" t="inlineStr">
-        <is>
-          <t>0775883247</t>
-        </is>
-      </c>
-      <c r="AA25" t="inlineStr">
-        <is>
-          <t>Luật sư</t>
-        </is>
-      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>Trần Tạ Minh</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>04/29/1986</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>0708160516</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>Nhà thiết kế đồ họa</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
@@ -3088,22 +3104,22 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Tạ Quốc</t>
+          <t>Trịnh Thành</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Mai</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>01/29/2004</t>
+          <t>12/15/2002</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -3113,22 +3129,22 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Khơ Mú</t>
+          <t>La Chi</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>09/25/2024</t>
+          <t>09/12/2024</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>0812096351</t>
+          <t>0933069477</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Đà Nẵng</t>
+          <t>Vĩnh Phúc</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -3138,7 +3154,7 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
@@ -3148,44 +3164,28 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Đặng Quách Quốc</t>
+          <t>Đặng Phan Thành</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>07/27/1962</t>
+          <t>10/14/1972</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>0787163175</t>
+          <t>0912205830</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Thư ký pháp lý</t>
-        </is>
-      </c>
-      <c r="T26" t="inlineStr">
-        <is>
-          <t>Đặng Khương Quốc</t>
-        </is>
-      </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>01/23/1960</t>
-        </is>
-      </c>
-      <c r="V26" t="inlineStr">
-        <is>
-          <t>0332734670</t>
-        </is>
-      </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>Công nhân sản xuất</t>
-        </is>
-      </c>
+          <t>Tư vấn khách hàng</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="inlineStr"/>
@@ -3205,47 +3205,47 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Chu Hữu</t>
+          <t>Đinh Hữu</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Lê</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>06/29/2004</t>
+          <t>03/29/2006</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Phù Lá</t>
+          <t>La Hu</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>09/01/2024</t>
+          <t>09/18/2024</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>0822500420</t>
+          <t>0753779027</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Hải Phòng</t>
+          <t>Đắk Nông</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -3265,42 +3265,42 @@
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Phạm Quách Thành</t>
+          <t>Phạm Khương Quốc</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>06/26/1968</t>
+          <t>06/15/1983</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>0720659164</t>
+          <t>0763902935</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Kiểm toán</t>
+          <t>Kiến trúc sư phần mềm</t>
         </is>
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>Trần Đinh Văn</t>
+          <t>Lê Phùng Hữu</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>04/27/1958</t>
+          <t>07/26/1973</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>0718565550</t>
+          <t>0988011843</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>Marketing Manager</t>
+          <t>Sales Representative</t>
         </is>
       </c>
       <c r="X27" t="inlineStr"/>
@@ -3322,22 +3322,22 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Võ Văn</t>
+          <t>Phí Đức</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Hoàng</t>
+          <t>Bùi</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>08/16/2000</t>
+          <t>04/16/2001</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -3347,27 +3347,27 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>M nông</t>
+          <t>Cờ Lao</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>09/18/2024</t>
+          <t>09/27/2024</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>0814981602</t>
+          <t>0304783858</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Bình Thuận</t>
+          <t>Phú Thọ</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -3380,28 +3380,44 @@
           <t>Không</t>
         </is>
       </c>
-      <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Đặng Trịnh Đình</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>05/05/1985</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>0389120250</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>Luật sư</t>
+        </is>
+      </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>Dương Võ Văn</t>
+          <t>Vũ Ngô Thành</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>04/12/1991</t>
+          <t>04/25/1992</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>0338898595</t>
+          <t>0356206224</t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
         <is>
-          <t>Sales Representative</t>
+          <t>DevOps Engineer</t>
         </is>
       </c>
       <c r="X28" t="inlineStr"/>
@@ -3423,47 +3439,47 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Lý Văn</t>
+          <t>Lưu Minh</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Hoàng</t>
+          <t>Dương</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>04/17/1999</t>
+          <t>01/30/2002</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Brau</t>
+          <t>Rơ Măm</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>09/25/2024</t>
+          <t>10/04/2024</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>0897056683</t>
+          <t>0306205276</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Ninh Thuận</t>
+          <t>Cà Mau</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -3473,7 +3489,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
@@ -3483,28 +3499,44 @@
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Mai Đào Hữu</t>
+          <t>Đặng Nguyễn Quốc</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>06/16/1964</t>
+          <t>02/10/1993</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>0822095475</t>
+          <t>0370408236</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Nhà thiết kế đồ họa</t>
-        </is>
-      </c>
-      <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
-      <c r="V29" t="inlineStr"/>
-      <c r="W29" t="inlineStr"/>
+          <t>Kỹ sư giám sát</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>Mai Đinh Thành</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>03/14/1974</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>0723842945</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>Nhân viên khách sạn</t>
+        </is>
+      </c>
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="inlineStr"/>
@@ -3524,22 +3556,22 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Đào Thành</t>
+          <t>Đào Hồng</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Nguyễn</t>
+          <t>Vũ</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>05/16/2004</t>
+          <t>05/15/2004</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -3549,32 +3581,32 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Pu Péo</t>
+          <t>Rơ Măm</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>09/02/2024</t>
+          <t>10/01/2024</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>0378289501</t>
+          <t>0973462606</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Hải Dương</t>
+          <t>Kon Tum</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
@@ -3582,30 +3614,30 @@
           <t>Không</t>
         </is>
       </c>
-      <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
-      <c r="T30" t="inlineStr">
-        <is>
-          <t>Mai Đào Thành</t>
-        </is>
-      </c>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>06/05/1958</t>
-        </is>
-      </c>
-      <c r="V30" t="inlineStr">
-        <is>
-          <t>0744894826</t>
-        </is>
-      </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>Kỹ sư nông nghiệp</t>
-        </is>
-      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Bùi Ngô Thành</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>07/05/1994</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>0358871070</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>Thư ký pháp lý</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" t="inlineStr"/>
@@ -3625,108 +3657,92 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Phan Thị</t>
+          <t>Hứa Đình</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Dương</t>
+          <t>Lê</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>01/31/2006</t>
+          <t>08/31/2001</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Chu Ru</t>
+          <t>Si La</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>09/23/2024</t>
+          <t>09/27/2024</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>0752476220</t>
+          <t>0969841551</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Quảng Bình</t>
+          <t>Hồ Chí Minh</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>Lê Thạch Thành</t>
-        </is>
-      </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>02/15/1974</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>0313121789</t>
-        </is>
-      </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>Giáo viên</t>
-        </is>
-      </c>
-      <c r="T31" t="inlineStr">
-        <is>
-          <t>Hoàng Vũ Quốc</t>
-        </is>
-      </c>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>07/04/1994</t>
-        </is>
-      </c>
-      <c r="V31" t="inlineStr">
-        <is>
-          <t>0812666480</t>
-        </is>
-      </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>Nông dân</t>
-        </is>
-      </c>
-      <c r="X31" t="inlineStr"/>
-      <c r="Y31" t="inlineStr"/>
-      <c r="Z31" t="inlineStr"/>
-      <c r="AA31" t="inlineStr"/>
+          <t>Ông bà</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>Mai Phí Hồng</t>
+        </is>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>10/20/1975</t>
+        </is>
+      </c>
+      <c r="Z31" t="inlineStr">
+        <is>
+          <t>0817200253</t>
+        </is>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>Lập trình viên</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
@@ -3742,47 +3758,47 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Trịnh Hữu</t>
+          <t>Trịnh Hồng</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Lê</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>07/13/2004</t>
+          <t>06/18/2003</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Phù Lá</t>
+          <t>Si La</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>09/14/2024</t>
+          <t>09/16/2024</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>0793300167</t>
+          <t>0738306860</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Lạng Sơn</t>
+          <t>Bình Dương</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
@@ -3806,22 +3822,22 @@
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr">
         <is>
-          <t>Bùi Đào Đức</t>
+          <t>Mai Phùng Quốc</t>
         </is>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>05/30/1994</t>
+          <t>12/29/1990</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>0896018046</t>
+          <t>0899278084</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>Nhà phân tích dữ liệu</t>
+          <t>Nhân viên khách sạn</t>
         </is>
       </c>
       <c r="X32" t="inlineStr"/>
@@ -3843,47 +3859,47 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Huỳnh Đức</t>
+          <t>Lê Thành</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Bùi</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>07/29/2003</t>
+          <t>04/22/2003</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Chứt</t>
+          <t>Gia Rai</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>09/09/2024</t>
+          <t>09/19/2024</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>0962960642</t>
+          <t>0336016986</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Sóc Trăng</t>
+          <t>Cần Thơ</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
@@ -3911,22 +3927,22 @@
       <c r="W33" t="inlineStr"/>
       <c r="X33" t="inlineStr">
         <is>
-          <t>Phạm Thái Thành</t>
+          <t>Hoàng Trịnh Thị</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>05/22/1971</t>
+          <t>10/01/1964</t>
         </is>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>0918717548</t>
+          <t>0324547945</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>Kỹ sư sản xuất</t>
+          <t>Giám đốc kinh doanh</t>
         </is>
       </c>
     </row>
@@ -3944,22 +3960,22 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Chu Thị</t>
+          <t>Trịnh Hồng</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Hoàng</t>
+          <t>Đặng</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>12/06/2004</t>
+          <t>11/15/2002</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -3969,83 +3985,67 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Cống</t>
+          <t>Chứt</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>09/21/2024</t>
+          <t>09/16/2024</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>0936605635</t>
+          <t>0772042516</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Lâm Đồng</t>
+          <t>Tây Ninh</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Không</t>
-        </is>
-      </c>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t>Bùi Hứa Thành</t>
-        </is>
-      </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>07/19/1992</t>
-        </is>
-      </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>0869661611</t>
-        </is>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>Nhân viên hành chính</t>
-        </is>
-      </c>
-      <c r="T34" t="inlineStr">
-        <is>
-          <t>Mai Trịnh Hữu</t>
-        </is>
-      </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>06/03/1989</t>
-        </is>
-      </c>
-      <c r="V34" t="inlineStr">
-        <is>
-          <t>0367346737</t>
-        </is>
-      </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>Chuyên viên bảo mật</t>
-        </is>
-      </c>
-      <c r="X34" t="inlineStr"/>
-      <c r="Y34" t="inlineStr"/>
-      <c r="Z34" t="inlineStr"/>
-      <c r="AA34" t="inlineStr"/>
+          <t>Họ hàng</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>Mai Hứa Hữu</t>
+        </is>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>10/07/1964</t>
+        </is>
+      </c>
+      <c r="Z34" t="inlineStr">
+        <is>
+          <t>0819190110</t>
+        </is>
+      </c>
+      <c r="AA34" t="inlineStr">
+        <is>
+          <t>Bác sĩ</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -4061,22 +4061,22 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Tôn Đức</t>
+          <t>Nguyễn Hữu</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Bùi</t>
+          <t>Nguyễn</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>09/20/2003</t>
+          <t>03/18/2002</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -4086,22 +4086,22 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Ro Mam</t>
+          <t>Phù Lá</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>09/17/2024</t>
+          <t>09/22/2024</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>0329028946</t>
+          <t>0345454352</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Cần Thơ</t>
+          <t>Vĩnh Long</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
@@ -4125,22 +4125,22 @@
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr">
         <is>
-          <t>Dương Trịnh Văn</t>
+          <t>Hoàng Khương Thành</t>
         </is>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>04/27/1977</t>
+          <t>06/02/1978</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>0909869073</t>
+          <t>0846700272</t>
         </is>
       </c>
       <c r="W35" t="inlineStr">
         <is>
-          <t>Quản lý sản xuất</t>
+          <t>Chuyên viên bán hàng trực tuyến</t>
         </is>
       </c>
       <c r="X35" t="inlineStr"/>
@@ -4162,22 +4162,22 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Đinh Quốc</t>
+          <t>Khương Thành</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Dương</t>
+          <t>Bùi</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>03/13/1999</t>
+          <t>05/25/2000</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -4187,27 +4187,27 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Khmer</t>
+          <t>Lô Lô</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>09/26/2024</t>
+          <t>09/29/2024</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>0924758606</t>
+          <t>0316440925</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Bà Rịa - Vũng Tàu</t>
+          <t>Trà Vinh</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -4220,28 +4220,44 @@
           <t>Không</t>
         </is>
       </c>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
-      <c r="S36" t="inlineStr"/>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>Hoàng Tôn Đức</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>08/09/1959</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>0303863965</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>Quản lý sản xuất</t>
+        </is>
+      </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>Đặng Sơn Văn</t>
+          <t>Trần Hồ Thành</t>
         </is>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>11/27/1979</t>
+          <t>01/20/1955</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>0934540271</t>
+          <t>0779577322</t>
         </is>
       </c>
       <c r="W36" t="inlineStr">
         <is>
-          <t>Nhân viên nhà hàng</t>
+          <t>Quản lý sản xuất</t>
         </is>
       </c>
       <c r="X36" t="inlineStr"/>
@@ -4263,22 +4279,22 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Hà Đức</t>
+          <t>Uông Minh</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Phạm</t>
+          <t>Bùi</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>11/30/2004</t>
+          <t>11/20/1999</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -4288,22 +4304,22 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Hoa</t>
+          <t>Ba Na</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>09/03/2024</t>
+          <t>10/09/2024</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>0821525390</t>
+          <t>0316768666</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Đắk Lắk</t>
+          <t>Bình Thuận</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
@@ -4313,7 +4329,7 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
@@ -4323,44 +4339,28 @@
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Hoàng Vương Đình</t>
+          <t>Hoàng Thạch Hữu</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>02/06/1963</t>
+          <t>08/05/1984</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>0727608499</t>
+          <t>0330751534</t>
         </is>
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Lập trình viên</t>
-        </is>
-      </c>
-      <c r="T37" t="inlineStr">
-        <is>
-          <t>Vũ Tạ Đức</t>
-        </is>
-      </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>04/14/1973</t>
-        </is>
-      </c>
-      <c r="V37" t="inlineStr">
-        <is>
-          <t>0982576491</t>
-        </is>
-      </c>
-      <c r="W37" t="inlineStr">
-        <is>
-          <t>Chuyên viên phân tích thị trường</t>
-        </is>
-      </c>
+          <t>Thợ xây</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr"/>
+      <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
       <c r="X37" t="inlineStr"/>
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" t="inlineStr"/>
@@ -4380,22 +4380,22 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Hà Quốc</t>
+          <t>Sơn Văn</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Hoàng</t>
+          <t>Vũ</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>08/27/2006</t>
+          <t>12/04/2002</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -4405,22 +4405,22 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Bố Y</t>
+          <t>Thái</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>09/12/2024</t>
+          <t>10/01/2024</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>0778215928</t>
+          <t>0980429513</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Trà Vinh</t>
+          <t>Bạc Liêu</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
@@ -4435,7 +4435,7 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Anh chị</t>
+          <t>Ông bà</t>
         </is>
       </c>
       <c r="P38" t="inlineStr"/>
@@ -4448,22 +4448,22 @@
       <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr">
         <is>
-          <t>Dương Vương Hồng</t>
+          <t>Lê Đoàn Minh</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
         <is>
-          <t>10/10/1953</t>
+          <t>09/07/1983</t>
         </is>
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>0322417553</t>
+          <t>0894014334</t>
         </is>
       </c>
       <c r="AA38" t="inlineStr">
         <is>
-          <t>Thợ xây</t>
+          <t>Chuyên viên bảo mật</t>
         </is>
       </c>
     </row>
@@ -4481,12 +4481,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Trịnh Văn</t>
+          <t>Quách Thị</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4496,32 +4496,32 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>03/31/2003</t>
+          <t>03/01/2001</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Sán Chay</t>
+          <t>Pu Péo</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>09/15/2024</t>
+          <t>09/28/2024</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>0927099421</t>
+          <t>0941936749</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Tiền Giang</t>
+          <t>Bình Thuận</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -4541,42 +4541,42 @@
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Trần Quách Quốc</t>
+          <t>Mai Phí Hữu</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>06/18/1990</t>
+          <t>08/25/1960</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>0790091345</t>
+          <t>0749308402</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Giáo viên</t>
+          <t>Digital Marketer</t>
         </is>
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>Lê Tôn Đức</t>
+          <t>Dương Thạch Văn</t>
         </is>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>09/12/1966</t>
+          <t>08/21/1962</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>0950251157</t>
+          <t>0914505332</t>
         </is>
       </c>
       <c r="W39" t="inlineStr">
         <is>
-          <t>Sales Representative</t>
+          <t>Giám đốc kinh doanh</t>
         </is>
       </c>
       <c r="X39" t="inlineStr"/>
@@ -4598,22 +4598,22 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Khương Đức</t>
+          <t>Vương Đình</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Hoàng</t>
+          <t>Phạm</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>01/26/2000</t>
+          <t>04/09/2000</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -4623,22 +4623,22 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Lô Lô</t>
+          <t>Brau</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>10/09/2024</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>0897601443</t>
+          <t>0399179156</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Thanh Hóa</t>
+          <t>Đồng Nai</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -4658,22 +4658,22 @@
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Trần Thạch Hồng</t>
+          <t>Dương Phí Hồng</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>04/01/1994</t>
+          <t>09/03/1977</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>0853505586</t>
+          <t>0972926106</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Nhà phân tích dữ liệu</t>
+          <t>Nhân viên nhà hàng</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
@@ -4699,47 +4699,47 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1A1</t>
+          <t>1A4</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Chu Đức</t>
+          <t>Tạ Thị</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Trần</t>
+          <t>Mai</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>01/21/2000</t>
+          <t>12/07/1998</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Mảng</t>
+          <t>Nùng</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>09/01/2024</t>
+          <t>09/24/2024</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>0727571601</t>
+          <t>0700353640</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Đắk Nông</t>
+          <t>Điện Biên</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
@@ -4749,42 +4749,42 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Họ hàng</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr"/>
-      <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
-      <c r="V41" t="inlineStr"/>
-      <c r="W41" t="inlineStr"/>
-      <c r="X41" t="inlineStr">
-        <is>
-          <t>Bùi Khương Văn</t>
-        </is>
-      </c>
-      <c r="Y41" t="inlineStr">
-        <is>
-          <t>05/12/1976</t>
-        </is>
-      </c>
-      <c r="Z41" t="inlineStr">
-        <is>
-          <t>0391995346</t>
-        </is>
-      </c>
-      <c r="AA41" t="inlineStr">
-        <is>
-          <t>Nông dân</t>
-        </is>
-      </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>Trần Trịnh Hữu</t>
+        </is>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>07/13/1977</t>
+        </is>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>0767801757</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>Lập trình viên</t>
+        </is>
+      </c>
+      <c r="X41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr"/>
+      <c r="Z41" t="inlineStr"/>
+      <c r="AA41" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>